<commit_message>
Add test coverage report, Docker deployment docs, and burndown chart
</commit_message>
<xml_diff>
--- a/scrum/Burndown Chart Template.xlsx
+++ b/scrum/Burndown Chart Template.xlsx
@@ -1,37 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://msudenver-my.sharepoint.com/personal/tmota_msudenver_edu/Documents/Teaching/Courses/__24SCS3250_SE/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e252ae034da6c357/Desktop/SWDEV2025/project-3-final-purple-t-pythons/scrum/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7397B228-E7AA-634C-96A5-F3624B942EAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="15" documentId="8_{7397B228-E7AA-634C-96A5-F3624B942EAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{61278168-8135-425D-AF2C-D1A87C41DE4E}"/>
   <bookViews>
-    <workbookView xWindow="1180" yWindow="1500" windowWidth="27240" windowHeight="15020" xr2:uid="{7A4C5A10-B1D5-9946-8D6C-7E3C0798020F}"/>
+    <workbookView xWindow="-760" yWindow="1080" windowWidth="19200" windowHeight="11170" xr2:uid="{7A4C5A10-B1D5-9946-8D6C-7E3C0798020F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$C$1:$G$1</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$C$2:$G$2</definedName>
-    <definedName name="_xlchart.v1.10" hidden="1">Sheet1!$C$3:$G$3</definedName>
-    <definedName name="_xlchart.v1.11" hidden="1">Sheet1!$C$1:$G$1</definedName>
-    <definedName name="_xlchart.v1.12" hidden="1">Sheet1!$C$2:$G$2</definedName>
-    <definedName name="_xlchart.v1.13" hidden="1">Sheet1!$C$3:$G$3</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Sheet1!$C$3:$G$3</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Sheet1!$C$4:$G$4</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">Sheet1!$C$1:$G$1</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">Sheet1!$C$2:$G$2</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">Sheet1!$C$3:$G$3</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">Sheet1!$C$4:$G$4</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">Sheet1!$C$1:$G$1</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">Sheet1!$C$2:$G$2</definedName>
-  </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -52,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Sprint 1</t>
   </si>
@@ -61,12 +45,6 @@
   </si>
   <si>
     <t>Sprint 3</t>
-  </si>
-  <si>
-    <t>Sprint 4</t>
-  </si>
-  <si>
-    <t>Sprint 5</t>
   </si>
   <si>
     <t>Planned</t>
@@ -290,7 +268,7 @@
             <c:strRef>
               <c:f>Sheet1!$C$1:$G$1</c:f>
               <c:strCache>
-                <c:ptCount val="5"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>Sprint 1</c:v>
                 </c:pt>
@@ -299,12 +277,6 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>Sprint 3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Sprint 4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Sprint 5</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -323,12 +295,6 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>80</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>40</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>40</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -359,7 +325,7 @@
             <c:strRef>
               <c:f>Sheet1!$C$1:$G$1</c:f>
               <c:strCache>
-                <c:ptCount val="5"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>Sprint 1</c:v>
                 </c:pt>
@@ -368,12 +334,6 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>Sprint 3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Sprint 4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Sprint 5</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -392,12 +352,6 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>65</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>50</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>40</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -448,19 +402,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>175</c:v>
+                  <c:v>-54</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>140</c:v>
+                  <c:v>-47</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>75</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>50</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>-78</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -497,18 +445,12 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>200</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>155</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>90</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>40</c:v>
-                </c:pt>
-                <c:pt idx="4">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -696,6 +638,7 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -703,7 +646,6 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -1325,9 +1267,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1365,7 +1307,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1471,7 +1413,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1613,7 +1555,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1623,19 +1565,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46ADD8F6-D520-684C-80D6-92D618A9A1CC}">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="2" width="11.6640625" style="1" customWidth="1"/>
     <col min="3" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B1" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>0</v>
@@ -1646,16 +1588,12 @@
       <c r="E1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2" s="3" t="s">
         <v>3</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
-        <v>5</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3">
@@ -1667,16 +1605,12 @@
       <c r="E2" s="3">
         <v>80</v>
       </c>
-      <c r="F2" s="3">
-        <v>40</v>
-      </c>
-      <c r="G2" s="3">
-        <v>40</v>
-      </c>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="4">
@@ -1688,66 +1622,47 @@
       <c r="E3" s="4">
         <v>65</v>
       </c>
-      <c r="F3" s="4">
-        <v>50</v>
-      </c>
-      <c r="G3" s="4">
-        <v>40</v>
-      </c>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="3">
         <f>B5-C2</f>
-        <v>175</v>
+        <v>-54</v>
       </c>
       <c r="D4" s="3">
         <f t="shared" ref="D4:G4" si="0">C5-D2</f>
-        <v>140</v>
+        <v>-47</v>
       </c>
       <c r="E4" s="3">
         <f t="shared" si="0"/>
-        <v>75</v>
-      </c>
-      <c r="F4" s="3">
-        <f t="shared" si="0"/>
-        <v>50</v>
-      </c>
-      <c r="G4" s="3">
-        <f t="shared" si="0"/>
+        <v>-78</v>
+      </c>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A5" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="4">
+        <v>21</v>
+      </c>
+      <c r="C5" s="4">
+        <v>13</v>
+      </c>
+      <c r="D5" s="4">
+        <v>2</v>
+      </c>
+      <c r="E5" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="4">
-        <v>250</v>
-      </c>
-      <c r="C5" s="4">
-        <f>B5-C3</f>
-        <v>200</v>
-      </c>
-      <c r="D5" s="4">
-        <f t="shared" ref="D5:G5" si="1">C5-D3</f>
-        <v>155</v>
-      </c>
-      <c r="E5" s="4">
-        <f t="shared" si="1"/>
-        <v>90</v>
-      </c>
-      <c r="F5" s="4">
-        <f t="shared" si="1"/>
-        <v>40</v>
-      </c>
-      <c r="G5" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>